<commit_message>
Separated 03-DifferentModels into 3 file
 - Cleaned the dataset code
 - Fixed the data preprocessing
 - Produced new graphs
</commit_message>
<xml_diff>
--- a/02-Cleaned_Dataset.xlsx
+++ b/02-Cleaned_Dataset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="299">
   <si>
     <t>Tweet</t>
   </si>
@@ -166,7 +166,7 @@
     <t>@xBFDR yeah I'm sure it will, it's just so depressing having to talk to my parents over the phone instead of talking to them downstairs</t>
   </si>
   <si>
-    <t>| At home sick... ðŸŽ¼The bluesðŸŽ¼ won't cure it so I need ideas ðŸŽ¸ðŸˁEE­ | #sorethroat #sick #blues #music #fallweather #carletonuniversity #ottawa</t>
+    <t>| At home sick... ðŸŽ¼The bluesðŸŽ¼ won't cure it so I need ideas ðŸŽ¸ðŸˁEEEE­ | #sorethroat #sick #blues #music #fallweather #carletonuniversity #ottawa</t>
   </si>
   <si>
     <t>I wouldn't wish anxiety and depression even on the worst of people. It's not fun. #anxiety #depression</t>
@@ -181,10 +181,10 @@
     <t>come to the funeral tomorrow at 12 to mourn the death of my gpa</t>
   </si>
   <si>
-    <t>Thought I had a pretty solid GPA as a kin major and now that I look at the average for dpt programs I feel even more discouraged ðŸˁEEª</t>
-  </si>
-  <si>
-    <t>depress ðŸˁEE</t>
+    <t>Thought I had a pretty solid GPA as a kin major and now that I look at the average for dpt programs I feel even more discouraged ðŸˁEEEEª</t>
+  </si>
+  <si>
+    <t>depress ðŸˁEEEE</t>
   </si>
   <si>
     <t>Summer officially ends today. #sadness</t>
@@ -214,7 +214,7 @@
     <t>Wearing all black tomorrow as I continue to mourn the lives of the most recent victims of police brutality. #blackout #WU</t>
   </si>
   <si>
-    <t>Am I the only person who dislikes fall? #FirstDayofFall #leaves #thingsdie #depressing #cold #noflipflops ðŸ�EE��EEŽðŸEE¾ðŸ�EE��EEŽðŸEE½ðŸ�EE��EEŽðŸEE»ðŸEE�EE��EEðŸ</t>
+    <t>Am I the only person who dislikes fall? #FirstDayofFall #leaves #thingsdie #depressing #cold #noflipflops ðŸ�EEEE��EEEEŽðŸEEEE¾ðŸ�EEEE��EEEEŽðŸEEEE½ðŸ�EEEE��EEEEŽðŸEEEE»ðŸEEEE�EEEE��EEEEðŸ</t>
   </si>
   <si>
     <t>My soul is weary of fighting the battles in this world. #BlackInAmerica #WeAreNotSafe</t>
@@ -253,22 +253,22 @@
     <t>@CTV_PowerPlay @lraitt Horrid disease! My maternal grandmother and each of her sisters suffered from this affliction. It's hard on all.</t>
   </si>
   <si>
-    <t>If anybody needs me I'll be drowning my blues in a sea of whiskey ðŸEE»</t>
-  </si>
-  <si>
-    <t>@Gaychel22 @Kellee_II @seattlepi even hard facts don't seem to be sinking in... I despair ðŸˁEE©</t>
+    <t>If anybody needs me I'll be drowning my blues in a sea of whiskey ðŸEEEE»</t>
+  </si>
+  <si>
+    <t>@Gaychel22 @Kellee_II @seattlepi even hard facts don't seem to be sinking in... I despair ðŸˁEEEE©</t>
   </si>
   <si>
     <t>So depressing that it's darker so much earlier now</t>
   </si>
   <si>
-    <t>It's just begun ladies and gents. The war on racism has begun. #sadness #Segregation continues.... smh ðŸˁEE�EE��EE</t>
+    <t>It's just begun ladies and gents. The war on racism has begun. #sadness #Segregation continues.... smh ðŸˁEEEE�EEEE��EEEE</t>
   </si>
   <si>
     <t>@ily_geuly call me now I'm laying in my bed moping like I intend to do for the next 2 months.</t>
   </si>
   <si>
-    <t>Baaarissshhhhh + sad song =  prefect night â�EE�EE��EE��EE feeling alone</t>
+    <t>Baaarissshhhhh + sad song =  prefect night â�EEEE�EEEE��EEEE��EEEE feeling alone</t>
   </si>
   <si>
     <t>im so gloomy today</t>
@@ -331,7 +331,7 @@
     <t>And there is despair underneath each and every action \nEach and every attempt to pierce the armour of numbness ' -Mgla</t>
   </si>
   <si>
-    <t>One step forward, two steps backward, the link to RogerFedererShop doesnÁEE´t work.ðŸˁEE° I am losing hope about Roger Federer new Website #sadness</t>
+    <t>One step forward, two steps backward, the link to RogerFedererShop doesnÁEEEE´t work.ðŸˁEEEE° I am losing hope about Roger Federer new Website #sadness</t>
   </si>
   <si>
     <t>My friends tell me I'm pretty. Trigger tells my I'm ugly. I first was confused but then realised I'm both. Pretty ugly. #tru  #tumblr</t>
@@ -415,7 +415,7 @@
     <t>Don't wanna go to work but I want the money #sad</t>
   </si>
   <si>
-    <t>Wow the #Denver housing market is #depressing no places to buy in my range ðŸˁEE¢ #FML</t>
+    <t>Wow the #Denver housing market is #depressing no places to buy in my range ðŸˁEEEE¢ #FML</t>
   </si>
   <si>
     <t>I have not nap for 3 days in a row I'm very unhappy rn</t>
@@ -481,7 +481,7 @@
     <t>@HutchinsonDave I don't know whether to despair or agitate for a cull.</t>
   </si>
   <si>
-    <t>Can I just sulk in peace ðŸˁEE�EE��EE</t>
+    <t>Can I just sulk in peace ðŸˁEEEE�EEEE��EEEE</t>
   </si>
   <si>
     <t>It's sad when your man leaves work a little bit late and your worst fear is 'Oh no!! Did he get stopped by the police?!?! ' #sad #ourworld</t>
@@ -538,7 +538,7 @@
     <t>@JUSTICESLUT420 sadly this sort of poster died by the 90s afaik</t>
   </si>
   <si>
-    <t>@lucy_hyner @Soulboy2266 sadly not !! One less hour drinking time ðŸˁEE¢ðŸEE»</t>
+    <t>@lucy_hyner @Soulboy2266 sadly not !! One less hour drinking time ðŸˁEEEE¢ðŸEEEE»</t>
   </si>
   <si>
     <t>I was in the dark room for 58 minutes and failed every time I tried developing a photo I'm so frustrated with myself :')</t>
@@ -607,7 +607,7 @@
     <t>@WestHamUtd poor service tonight to find season ticket holders in the seats we purchased online. Forced to move further away #unhappy</t>
   </si>
   <si>
-    <t>Even a pencilâŁEEEE never #stayed  with me until it's #end âš« ðŸˁEEž</t>
+    <t>Even a pencilâŁEEEEEEEE never #stayed  with me until it's #end âš« ðŸˁEEEEž</t>
   </si>
   <si>
     <t>so gutted i dropped one of my earrings down the sink at school</t>
@@ -625,10 +625,10 @@
     <t>All the 'juniors' are now wearing purple at ollafest while I'm here fighting with my alarm about when I need to wake up for German #sadness</t>
   </si>
   <si>
-    <t>The fact I haven't had to wear a bra for a week and knowing I'll have to start wearing one again after tomorrow is depressing ðŸ�EE�EE��EE��EEðŸ�EE�EE��EE��EE</t>
-  </si>
-  <si>
-    <t>Liam is too distant makes me mourn ðŸˁEEª</t>
+    <t>The fact I haven't had to wear a bra for a week and knowing I'll have to start wearing one again after tomorrow is depressing ðŸ�EEEE�EEEE��EEEE��EEEEðŸ�EEEE�EEEE��EEEE��EEEE</t>
+  </si>
+  <si>
+    <t>Liam is too distant makes me mourn ðŸˁEEEEª</t>
   </si>
   <si>
     <t>It's now September and we're still battling a situation that was said to be handled March of this year. @ATT this is unacceptable</t>
@@ -814,7 +814,7 @@
     <t>@ChibiReviews Post series depression can be quite bad, but it will get better, I bet someone will pick the novel soon in the west.</t>
   </si>
   <si>
-    <t>@iTriborg â�EE�EE��EE��EE make him feel vigorous. 'Fine. You can kill me now.' Said Hestia with a display of only despair rather than her joyful â�EE�EE��EE��EE</t>
+    <t>@iTriborg â�EEEE�EEEE��EEEE��EEEE make him feel vigorous. 'Fine. You can kill me now.' Said Hestia with a display of only despair rather than her joyful â�EEEE�EEEE��EEEE��EEEE</t>
   </si>
   <si>
     <t>The 2nd step to beating #anxiety or #depression is realising that it's not about waiting for ...., Take action yourself now.</t>
@@ -850,7 +850,7 @@
     <t>In need of a serious nap rn</t>
   </si>
   <si>
-    <t>@JohnWildy71 something, too confused to type an entire word ðŸˁEEŁEE See, I can laugh again. My hour of sadness has almost passed</t>
+    <t>@JohnWildy71 something, too confused to type an entire word ðŸˁEEEEŁEEEE See, I can laugh again. My hour of sadness has almost passed</t>
   </si>
   <si>
     <t>Interview preparation, I hate talking about myself, one dull subject matter! #yawnoff</t>
@@ -862,7 +862,7 @@
     <t>No episode today! Whilst editing there was a power outage! We will rebuild...tomorrow #podcast #lost #editing #fail #tomorrow</t>
   </si>
   <si>
-    <t>It is a solemn thing, and no small scandal in the Kingdom, to see Godâ�EE�EE��EE�EE�s children starving while seated at the Fatherâ�EE�EE��EE�EE�s table. -AW Tozer</t>
+    <t>It is a solemn thing, and no small scandal in the Kingdom, to see Godâ�EEEE�EEEE��EEEE�EEEE�s children starving while seated at the Fatherâ�EEEE�EEEE��EEEE�EEEE�s table. -AW Tozer</t>
   </si>
   <si>
     <t>Gonna be a loooooong year as a Browns fan. Longer than normal and that's</t>
@@ -883,7 +883,7 @@
     <t>Pops are joyless, soulless toys which look nearly identical.  They are the perfect expression of consumerism.  'I enjoy this franchise'</t>
   </si>
   <si>
-    <t>Why is it that we rejoice at a birth and grieve at a funeral? It is because we are not the person involved. â�EE�EE��EE�� Mark Twain</t>
+    <t>Why is it that we rejoice at a birth and grieve at a funeral? It is because we are not the person involved. â�EEEE�EEEE��EEEE�� Mark Twain</t>
   </si>
   <si>
     <t>Regret for the things we did can be tempered by time; it is regret for the things we did not do that is inconsolable. - Sydney J. Harris</t>
@@ -911,30 +911,6 @@
   </si>
   <si>
     <t>guilty</t>
-  </si>
-  <si>
-    <t>guilt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lonely </t>
-  </si>
-  <si>
-    <t xml:space="preserve">depressed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">displeased </t>
-  </si>
-  <si>
-    <t xml:space="preserve">grief </t>
-  </si>
-  <si>
-    <t xml:space="preserve">guilt </t>
-  </si>
-  <si>
-    <t>lost</t>
-  </si>
-  <si>
-    <t>depression</t>
   </si>
 </sst>
 </file>
@@ -2739,7 +2715,7 @@
         <v>3</v>
       </c>
       <c r="P35" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="Q35">
         <v>3</v>
@@ -5767,7 +5743,7 @@
         <v>5</v>
       </c>
       <c r="N109" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O109">
         <v>3</v>
@@ -5796,7 +5772,7 @@
         <v>5</v>
       </c>
       <c r="N110" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O110">
         <v>4</v>
@@ -5825,7 +5801,7 @@
         <v>1</v>
       </c>
       <c r="N111" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O111">
         <v>4</v>
@@ -5854,7 +5830,7 @@
         <v>4</v>
       </c>
       <c r="N112" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O112">
         <v>4</v>
@@ -5883,7 +5859,7 @@
         <v>4</v>
       </c>
       <c r="N113" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O113">
         <v>4</v>
@@ -5912,7 +5888,7 @@
         <v>2</v>
       </c>
       <c r="N114" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O114">
         <v>3</v>
@@ -5941,7 +5917,7 @@
         <v>2</v>
       </c>
       <c r="N115" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O115">
         <v>2</v>
@@ -5970,7 +5946,7 @@
         <v>3</v>
       </c>
       <c r="N116" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O116">
         <v>3</v>
@@ -6028,7 +6004,7 @@
         <v>1</v>
       </c>
       <c r="N118" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O118">
         <v>3</v>
@@ -6057,7 +6033,7 @@
         <v>1</v>
       </c>
       <c r="N119" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O119">
         <v>3</v>
@@ -6086,7 +6062,7 @@
         <v>3</v>
       </c>
       <c r="N120" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O120">
         <v>4</v>
@@ -6173,7 +6149,7 @@
         <v>1</v>
       </c>
       <c r="N123" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O123">
         <v>4</v>
@@ -6202,7 +6178,7 @@
         <v>3</v>
       </c>
       <c r="N124" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O124">
         <v>3</v>
@@ -6231,7 +6207,7 @@
         <v>2</v>
       </c>
       <c r="N125" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O125">
         <v>3</v>
@@ -6260,7 +6236,7 @@
         <v>4</v>
       </c>
       <c r="N126" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="O126">
         <v>4</v>
@@ -6289,7 +6265,7 @@
         <v>1</v>
       </c>
       <c r="N127" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O127">
         <v>3</v>
@@ -6347,7 +6323,7 @@
         <v>1</v>
       </c>
       <c r="N129" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O129">
         <v>4</v>
@@ -6376,7 +6352,7 @@
         <v>2</v>
       </c>
       <c r="N130" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O130">
         <v>4</v>
@@ -6405,7 +6381,7 @@
         <v>5</v>
       </c>
       <c r="N131" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O131">
         <v>5</v>
@@ -6434,7 +6410,7 @@
         <v>3</v>
       </c>
       <c r="N132" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O132">
         <v>3</v>
@@ -6463,7 +6439,7 @@
         <v>3</v>
       </c>
       <c r="N133" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O133">
         <v>3</v>
@@ -6492,7 +6468,7 @@
         <v>1</v>
       </c>
       <c r="N134" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O134">
         <v>4</v>
@@ -6521,7 +6497,7 @@
         <v>1</v>
       </c>
       <c r="N135" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O135">
         <v>3</v>
@@ -6550,7 +6526,7 @@
         <v>1</v>
       </c>
       <c r="N136" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O136">
         <v>3</v>
@@ -6579,7 +6555,7 @@
         <v>3</v>
       </c>
       <c r="N137" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O137">
         <v>3</v>
@@ -6608,7 +6584,7 @@
         <v>3</v>
       </c>
       <c r="N138" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O138">
         <v>3</v>
@@ -6637,7 +6613,7 @@
         <v>1</v>
       </c>
       <c r="N139" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O139">
         <v>3</v>
@@ -6666,7 +6642,7 @@
         <v>3</v>
       </c>
       <c r="N140" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O140">
         <v>3</v>
@@ -6695,7 +6671,7 @@
         <v>3</v>
       </c>
       <c r="N141" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O141">
         <v>4</v>
@@ -6724,7 +6700,7 @@
         <v>1</v>
       </c>
       <c r="N142" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O142">
         <v>3</v>
@@ -6753,7 +6729,7 @@
         <v>1</v>
       </c>
       <c r="N143" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O143">
         <v>3</v>
@@ -6782,7 +6758,7 @@
         <v>2</v>
       </c>
       <c r="N144" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O144">
         <v>3</v>
@@ -6811,7 +6787,7 @@
         <v>2</v>
       </c>
       <c r="N145" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O145">
         <v>3</v>
@@ -6840,7 +6816,7 @@
         <v>1</v>
       </c>
       <c r="N146" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O146">
         <v>4</v>
@@ -6869,7 +6845,7 @@
         <v>1</v>
       </c>
       <c r="N147" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O147">
         <v>2</v>
@@ -6898,7 +6874,7 @@
         <v>2</v>
       </c>
       <c r="N148" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O148">
         <v>1</v>
@@ -6927,7 +6903,7 @@
         <v>1</v>
       </c>
       <c r="N149" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="O149">
         <v>2</v>
@@ -6956,7 +6932,7 @@
         <v>1</v>
       </c>
       <c r="N150" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O150">
         <v>5</v>
@@ -6985,7 +6961,7 @@
         <v>3</v>
       </c>
       <c r="N151" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O151">
         <v>4</v>
@@ -7014,7 +6990,7 @@
         <v>2</v>
       </c>
       <c r="N152" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O152">
         <v>3</v>
@@ -7043,7 +7019,7 @@
         <v>2</v>
       </c>
       <c r="N153" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O153">
         <v>4</v>
@@ -7072,7 +7048,7 @@
         <v>2</v>
       </c>
       <c r="N154" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O154">
         <v>3</v>
@@ -7101,7 +7077,7 @@
         <v>2</v>
       </c>
       <c r="N155" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O155">
         <v>3</v>
@@ -7130,7 +7106,7 @@
         <v>1</v>
       </c>
       <c r="N156" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O156">
         <v>2</v>
@@ -7159,7 +7135,7 @@
         <v>1</v>
       </c>
       <c r="N157" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O157">
         <v>2</v>
@@ -7188,7 +7164,7 @@
         <v>2</v>
       </c>
       <c r="N158" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O158">
         <v>4</v>
@@ -7217,7 +7193,7 @@
         <v>3</v>
       </c>
       <c r="N159" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="O159">
         <v>3</v>
@@ -7246,7 +7222,7 @@
         <v>2</v>
       </c>
       <c r="N160" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="O160">
         <v>4</v>
@@ -7275,7 +7251,7 @@
         <v>1</v>
       </c>
       <c r="N161" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O161">
         <v>3</v>
@@ -7304,7 +7280,7 @@
         <v>2</v>
       </c>
       <c r="N162" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O162">
         <v>5</v>
@@ -7333,7 +7309,7 @@
         <v>1</v>
       </c>
       <c r="N163" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O163">
         <v>3</v>
@@ -7362,7 +7338,7 @@
         <v>3</v>
       </c>
       <c r="N164" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O164">
         <v>5</v>
@@ -7391,7 +7367,7 @@
         <v>1</v>
       </c>
       <c r="N165" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O165">
         <v>3</v>
@@ -7420,7 +7396,7 @@
         <v>2</v>
       </c>
       <c r="N166" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O166">
         <v>4</v>
@@ -7449,7 +7425,7 @@
         <v>1</v>
       </c>
       <c r="N167" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O167">
         <v>2</v>
@@ -7478,7 +7454,7 @@
         <v>2</v>
       </c>
       <c r="N168" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O168">
         <v>5</v>
@@ -7507,7 +7483,7 @@
         <v>2</v>
       </c>
       <c r="N169" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O169">
         <v>3</v>
@@ -7536,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N170" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O170">
         <v>2</v>
@@ -7565,7 +7541,7 @@
         <v>2</v>
       </c>
       <c r="N171" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O171">
         <v>4</v>
@@ -7594,7 +7570,7 @@
         <v>2</v>
       </c>
       <c r="N172" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O172">
         <v>5</v>
@@ -7623,7 +7599,7 @@
         <v>1</v>
       </c>
       <c r="N173" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O173">
         <v>2</v>
@@ -7652,7 +7628,7 @@
         <v>1</v>
       </c>
       <c r="N174" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O174">
         <v>2</v>
@@ -7681,7 +7657,7 @@
         <v>1</v>
       </c>
       <c r="N175" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O175">
         <v>4</v>
@@ -7710,7 +7686,7 @@
         <v>3</v>
       </c>
       <c r="N176" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O176">
         <v>5</v>
@@ -7739,7 +7715,7 @@
         <v>2</v>
       </c>
       <c r="N177" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O177">
         <v>4</v>
@@ -7768,7 +7744,7 @@
         <v>3</v>
       </c>
       <c r="N178" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O178">
         <v>3</v>
@@ -7797,7 +7773,7 @@
         <v>2</v>
       </c>
       <c r="N179" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O179">
         <v>5</v>
@@ -7826,7 +7802,7 @@
         <v>1</v>
       </c>
       <c r="N180" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O180">
         <v>3</v>
@@ -7855,7 +7831,7 @@
         <v>2</v>
       </c>
       <c r="N181" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O181">
         <v>4</v>
@@ -7884,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="N182" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O182">
         <v>4</v>
@@ -7942,7 +7918,7 @@
         <v>4</v>
       </c>
       <c r="N184" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O184">
         <v>2</v>
@@ -7971,7 +7947,7 @@
         <v>2</v>
       </c>
       <c r="N185" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O185">
         <v>3</v>
@@ -8000,7 +7976,7 @@
         <v>1</v>
       </c>
       <c r="N186" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O186">
         <v>2</v>
@@ -8029,7 +8005,7 @@
         <v>2</v>
       </c>
       <c r="N187" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O187">
         <v>4</v>
@@ -8058,7 +8034,7 @@
         <v>3</v>
       </c>
       <c r="N188" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O188">
         <v>5</v>
@@ -8087,7 +8063,7 @@
         <v>2</v>
       </c>
       <c r="N189" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O189">
         <v>3</v>
@@ -8116,7 +8092,7 @@
         <v>2</v>
       </c>
       <c r="N190" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O190">
         <v>5</v>
@@ -8145,7 +8121,7 @@
         <v>2</v>
       </c>
       <c r="N191" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O191">
         <v>1</v>
@@ -8174,7 +8150,7 @@
         <v>2</v>
       </c>
       <c r="N192" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O192">
         <v>3</v>
@@ -8203,7 +8179,7 @@
         <v>1</v>
       </c>
       <c r="N193" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O193">
         <v>2</v>
@@ -8232,7 +8208,7 @@
         <v>3</v>
       </c>
       <c r="N194" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O194">
         <v>3</v>
@@ -8261,7 +8237,7 @@
         <v>1</v>
       </c>
       <c r="N195" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O195">
         <v>2</v>
@@ -8290,7 +8266,7 @@
         <v>2</v>
       </c>
       <c r="N196" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O196">
         <v>3</v>
@@ -8319,7 +8295,7 @@
         <v>1</v>
       </c>
       <c r="N197" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O197">
         <v>2</v>
@@ -8348,7 +8324,7 @@
         <v>3</v>
       </c>
       <c r="N198" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O198">
         <v>3</v>
@@ -8377,7 +8353,7 @@
         <v>2</v>
       </c>
       <c r="N199" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O199">
         <v>2</v>
@@ -8406,7 +8382,7 @@
         <v>1</v>
       </c>
       <c r="N200" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="O200">
         <v>1</v>
@@ -8435,7 +8411,7 @@
         <v>2</v>
       </c>
       <c r="N201" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O201">
         <v>5</v>
@@ -8464,7 +8440,7 @@
         <v>2</v>
       </c>
       <c r="N202" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O202">
         <v>4</v>
@@ -8522,7 +8498,7 @@
         <v>3</v>
       </c>
       <c r="N204" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O204">
         <v>5</v>
@@ -8551,7 +8527,7 @@
         <v>2</v>
       </c>
       <c r="N205" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O205">
         <v>5</v>
@@ -8580,7 +8556,7 @@
         <v>3</v>
       </c>
       <c r="N206" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O206">
         <v>3</v>
@@ -8609,7 +8585,7 @@
         <v>2</v>
       </c>
       <c r="N207" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O207">
         <v>3</v>

</xml_diff>